<commit_message>
Add new result images and statistical analysis files for classification and TSP algorithms
- Added fitness accuracy, speedup, and time vs size plots for ACO, GA, and PSO in classification results.
- Included fitness accuracy lines for cluster algorithms.
- Introduced new fitness gap comparison images for various TSP instances across ACO, GA, and PSO.
- Added statistical analysis Excel files for both classification and TSP results.
- Updated summary Excel files for classification and TSP cluster results.
</commit_message>
<xml_diff>
--- a/results/tsp_results_summary.xlsx
+++ b/results/tsp_results_summary.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ga_60s" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ga_1000it" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="aco_60s" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="aco_1000it" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="pso_60s" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="pso_1000it" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ga_60s" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ga_500it" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ga_1000it" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="aco_60s" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="aco_500it" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="aco_1000it" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pso_60s" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pso_500it" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pso_1000it" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1139,7 +1142,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1150,18 +1153,18 @@
         <v>29</v>
       </c>
       <c r="D2" t="n">
-        <v>2080</v>
+        <v>2107</v>
       </c>
       <c r="E2" t="n">
-        <v>2.97</v>
+        <v>4.31</v>
       </c>
       <c r="F2" t="n">
-        <v>21.75</v>
+        <v>10.94</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1178,12 +1181,12 @@
         <v>4.5</v>
       </c>
       <c r="F3" t="n">
-        <v>22.21</v>
+        <v>11.05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1200,12 +1203,12 @@
         <v>6.83</v>
       </c>
       <c r="F4" t="n">
-        <v>23.37</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1216,18 +1219,18 @@
         <v>76</v>
       </c>
       <c r="D5" t="n">
-        <v>575.2809448242188</v>
+        <v>580.4423828125</v>
       </c>
       <c r="E5" t="n">
-        <v>5.48</v>
+        <v>6.43</v>
       </c>
       <c r="F5" t="n">
-        <v>23.67</v>
+        <v>11.81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1238,18 +1241,18 @@
         <v>101</v>
       </c>
       <c r="D6" t="n">
-        <v>715.1535034179688</v>
+        <v>740.8201293945312</v>
       </c>
       <c r="E6" t="n">
-        <v>11.34</v>
+        <v>15.34</v>
       </c>
       <c r="F6" t="n">
-        <v>24.27</v>
+        <v>12.15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1260,18 +1263,18 @@
         <v>225</v>
       </c>
       <c r="D7" t="n">
-        <v>5460.66943359375</v>
+        <v>7533.8984375</v>
       </c>
       <c r="E7" t="n">
-        <v>41.5</v>
+        <v>95.23</v>
       </c>
       <c r="F7" t="n">
-        <v>26.75</v>
+        <v>13.47</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1282,18 +1285,18 @@
         <v>442</v>
       </c>
       <c r="D8" t="n">
-        <v>145242.828125</v>
+        <v>216009.359375</v>
       </c>
       <c r="E8" t="n">
-        <v>186</v>
+        <v>325.35</v>
       </c>
       <c r="F8" t="n">
-        <v>34.15</v>
+        <v>17.17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1310,12 +1313,12 @@
         <v>2.97</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1326,18 +1329,18 @@
         <v>51</v>
       </c>
       <c r="D10" t="n">
-        <v>462.7006530761719</v>
+        <v>467.2942810058594</v>
       </c>
       <c r="E10" t="n">
-        <v>7.61</v>
+        <v>8.68</v>
       </c>
       <c r="F10" t="n">
-        <v>1.05</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1348,18 +1351,18 @@
         <v>52</v>
       </c>
       <c r="D11" t="n">
-        <v>8223.33203125</v>
+        <v>8535.8857421875</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>13.14</v>
       </c>
       <c r="F11" t="n">
-        <v>1.09</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1370,18 +1373,18 @@
         <v>76</v>
       </c>
       <c r="D12" t="n">
-        <v>602.2460327148438</v>
+        <v>696.4586791992188</v>
       </c>
       <c r="E12" t="n">
-        <v>10.43</v>
+        <v>27.7</v>
       </c>
       <c r="F12" t="n">
-        <v>0.91</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1392,18 +1395,18 @@
         <v>101</v>
       </c>
       <c r="D13" t="n">
-        <v>765.7063598632812</v>
+        <v>844.6394653320312</v>
       </c>
       <c r="E13" t="n">
-        <v>19.21</v>
+        <v>31.5</v>
       </c>
       <c r="F13" t="n">
-        <v>0.92</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1414,18 +1417,18 @@
         <v>225</v>
       </c>
       <c r="D14" t="n">
-        <v>9699.3623046875</v>
+        <v>11343.859375</v>
       </c>
       <c r="E14" t="n">
-        <v>151.34</v>
+        <v>193.96</v>
       </c>
       <c r="F14" t="n">
-        <v>1.36</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1436,18 +1439,18 @@
         <v>442</v>
       </c>
       <c r="D15" t="n">
-        <v>221479.34375</v>
+        <v>262082.90625</v>
       </c>
       <c r="E15" t="n">
-        <v>336.12</v>
+        <v>416.08</v>
       </c>
       <c r="F15" t="n">
-        <v>1.38</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1464,12 +1467,12 @@
         <v>2.97</v>
       </c>
       <c r="F16" t="n">
-        <v>1.1</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1480,18 +1483,18 @@
         <v>51</v>
       </c>
       <c r="D17" t="n">
-        <v>462.7006530761719</v>
+        <v>467.2942810058594</v>
       </c>
       <c r="E17" t="n">
-        <v>7.61</v>
+        <v>8.68</v>
       </c>
       <c r="F17" t="n">
-        <v>1.11</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1502,18 +1505,18 @@
         <v>52</v>
       </c>
       <c r="D18" t="n">
-        <v>8223.33203125</v>
+        <v>8535.8857421875</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>13.14</v>
       </c>
       <c r="F18" t="n">
-        <v>1.45</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1524,18 +1527,18 @@
         <v>76</v>
       </c>
       <c r="D19" t="n">
-        <v>602.2460327148438</v>
+        <v>696.4586791992188</v>
       </c>
       <c r="E19" t="n">
-        <v>10.43</v>
+        <v>27.7</v>
       </c>
       <c r="F19" t="n">
-        <v>1.26</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1546,18 +1549,18 @@
         <v>101</v>
       </c>
       <c r="D20" t="n">
-        <v>765.7063598632812</v>
+        <v>844.6394653320312</v>
       </c>
       <c r="E20" t="n">
-        <v>19.21</v>
+        <v>31.5</v>
       </c>
       <c r="F20" t="n">
-        <v>1.18</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1568,18 +1571,18 @@
         <v>225</v>
       </c>
       <c r="D21" t="n">
-        <v>9699.3623046875</v>
+        <v>11343.859375</v>
       </c>
       <c r="E21" t="n">
-        <v>151.34</v>
+        <v>193.96</v>
       </c>
       <c r="F21" t="n">
-        <v>1.67</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1590,18 +1593,18 @@
         <v>442</v>
       </c>
       <c r="D22" t="n">
-        <v>221479.34375</v>
+        <v>262082.90625</v>
       </c>
       <c r="E22" t="n">
-        <v>336.12</v>
+        <v>416.08</v>
       </c>
       <c r="F22" t="n">
-        <v>1.94</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1618,12 +1621,12 @@
         <v>2.97</v>
       </c>
       <c r="F23" t="n">
-        <v>1.13</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1634,18 +1637,18 @@
         <v>51</v>
       </c>
       <c r="D24" t="n">
-        <v>462.7006530761719</v>
+        <v>467.2942810058594</v>
       </c>
       <c r="E24" t="n">
-        <v>7.61</v>
+        <v>8.68</v>
       </c>
       <c r="F24" t="n">
-        <v>1.16</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1656,18 +1659,18 @@
         <v>52</v>
       </c>
       <c r="D25" t="n">
-        <v>8223.33203125</v>
+        <v>8535.8857421875</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>13.14</v>
       </c>
       <c r="F25" t="n">
-        <v>1.06</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1678,18 +1681,18 @@
         <v>76</v>
       </c>
       <c r="D26" t="n">
-        <v>602.2460327148438</v>
+        <v>696.4586791992188</v>
       </c>
       <c r="E26" t="n">
-        <v>10.43</v>
+        <v>27.7</v>
       </c>
       <c r="F26" t="n">
-        <v>1.16</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1700,18 +1703,18 @@
         <v>101</v>
       </c>
       <c r="D27" t="n">
-        <v>765.7063598632812</v>
+        <v>844.6394653320312</v>
       </c>
       <c r="E27" t="n">
-        <v>19.21</v>
+        <v>31.5</v>
       </c>
       <c r="F27" t="n">
-        <v>1.37</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1722,18 +1725,18 @@
         <v>225</v>
       </c>
       <c r="D28" t="n">
-        <v>9699.3623046875</v>
+        <v>11343.859375</v>
       </c>
       <c r="E28" t="n">
-        <v>151.34</v>
+        <v>193.96</v>
       </c>
       <c r="F28" t="n">
-        <v>1.66</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1744,13 +1747,13 @@
         <v>442</v>
       </c>
       <c r="D29" t="n">
-        <v>221479.34375</v>
+        <v>262082.90625</v>
       </c>
       <c r="E29" t="n">
-        <v>336.12</v>
+        <v>416.08</v>
       </c>
       <c r="F29" t="n">
-        <v>2.02</v>
+        <v>1.45</v>
       </c>
     </row>
   </sheetData>
@@ -1775,7 +1778,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Timelimit</t>
+          <t>Iterations</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1806,7 +1809,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1817,18 +1820,18 @@
         <v>29</v>
       </c>
       <c r="D2" t="n">
-        <v>2020</v>
+        <v>2080</v>
       </c>
       <c r="E2" t="n">
-        <v>-0</v>
+        <v>2.97</v>
       </c>
       <c r="F2" t="n">
-        <v>60.01</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1839,18 +1842,18 @@
         <v>51</v>
       </c>
       <c r="D3" t="n">
-        <v>438.7414245605469</v>
+        <v>449.3215026855469</v>
       </c>
       <c r="E3" t="n">
-        <v>2.04</v>
+        <v>4.5</v>
       </c>
       <c r="F3" t="n">
-        <v>60.06</v>
+        <v>22.21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1861,18 +1864,18 @@
         <v>52</v>
       </c>
       <c r="D4" t="n">
-        <v>7548.9931640625</v>
+        <v>8059.57763671875</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06</v>
+        <v>6.83</v>
       </c>
       <c r="F4" t="n">
-        <v>60.01</v>
+        <v>23.37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1883,18 +1886,18 @@
         <v>76</v>
       </c>
       <c r="D5" t="n">
-        <v>555.097900390625</v>
+        <v>575.2809448242188</v>
       </c>
       <c r="E5" t="n">
-        <v>1.78</v>
+        <v>5.48</v>
       </c>
       <c r="F5" t="n">
-        <v>60.1</v>
+        <v>23.67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1905,18 +1908,18 @@
         <v>101</v>
       </c>
       <c r="D6" t="n">
-        <v>679.5157470703125</v>
+        <v>715.1535034179688</v>
       </c>
       <c r="E6" t="n">
-        <v>5.79</v>
+        <v>11.34</v>
       </c>
       <c r="F6" t="n">
-        <v>60.16</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1927,18 +1930,18 @@
         <v>225</v>
       </c>
       <c r="D7" t="n">
-        <v>4190.5361328125</v>
+        <v>5460.66943359375</v>
       </c>
       <c r="E7" t="n">
-        <v>8.59</v>
+        <v>41.5</v>
       </c>
       <c r="F7" t="n">
-        <v>60.49</v>
+        <v>26.75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1949,18 +1952,18 @@
         <v>442</v>
       </c>
       <c r="D8" t="n">
-        <v>62575.59375</v>
+        <v>145242.828125</v>
       </c>
       <c r="E8" t="n">
-        <v>23.22</v>
+        <v>186</v>
       </c>
       <c r="F8" t="n">
-        <v>62.53</v>
+        <v>34.15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1971,18 +1974,18 @@
         <v>29</v>
       </c>
       <c r="D9" t="n">
-        <v>2020</v>
+        <v>2080</v>
       </c>
       <c r="E9" t="n">
-        <v>-0</v>
+        <v>2.97</v>
       </c>
       <c r="F9" t="n">
-        <v>60</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1993,18 +1996,18 @@
         <v>51</v>
       </c>
       <c r="D10" t="n">
-        <v>432.6891784667969</v>
+        <v>462.7006530761719</v>
       </c>
       <c r="E10" t="n">
-        <v>0.63</v>
+        <v>7.61</v>
       </c>
       <c r="F10" t="n">
-        <v>60</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -2015,18 +2018,18 @@
         <v>52</v>
       </c>
       <c r="D11" t="n">
-        <v>7544.36572265625</v>
+        <v>8223.33203125</v>
       </c>
       <c r="E11" t="n">
-        <v>-0</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
-        <v>60</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -2037,18 +2040,18 @@
         <v>76</v>
       </c>
       <c r="D12" t="n">
-        <v>553.6527099609375</v>
+        <v>602.2460327148438</v>
       </c>
       <c r="E12" t="n">
-        <v>1.52</v>
+        <v>10.43</v>
       </c>
       <c r="F12" t="n">
-        <v>60</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -2059,18 +2062,18 @@
         <v>101</v>
       </c>
       <c r="D13" t="n">
-        <v>672.9217529296875</v>
+        <v>765.7063598632812</v>
       </c>
       <c r="E13" t="n">
-        <v>4.77</v>
+        <v>19.21</v>
       </c>
       <c r="F13" t="n">
-        <v>60.01</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -2081,18 +2084,18 @@
         <v>225</v>
       </c>
       <c r="D14" t="n">
-        <v>4142.7646484375</v>
+        <v>9699.3623046875</v>
       </c>
       <c r="E14" t="n">
-        <v>7.35</v>
+        <v>151.34</v>
       </c>
       <c r="F14" t="n">
-        <v>60.04</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -2103,18 +2106,18 @@
         <v>442</v>
       </c>
       <c r="D15" t="n">
-        <v>58054.23046875</v>
+        <v>221479.34375</v>
       </c>
       <c r="E15" t="n">
-        <v>14.32</v>
+        <v>336.12</v>
       </c>
       <c r="F15" t="n">
-        <v>60.19</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -2125,18 +2128,18 @@
         <v>29</v>
       </c>
       <c r="D16" t="n">
-        <v>2020</v>
+        <v>2080</v>
       </c>
       <c r="E16" t="n">
-        <v>-0</v>
+        <v>2.97</v>
       </c>
       <c r="F16" t="n">
-        <v>60</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -2147,18 +2150,18 @@
         <v>51</v>
       </c>
       <c r="D17" t="n">
-        <v>433.9072570800781</v>
+        <v>462.7006530761719</v>
       </c>
       <c r="E17" t="n">
-        <v>0.91</v>
+        <v>7.61</v>
       </c>
       <c r="F17" t="n">
-        <v>60</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -2169,18 +2172,18 @@
         <v>52</v>
       </c>
       <c r="D18" t="n">
-        <v>7544.6630859375</v>
+        <v>8223.33203125</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
-        <v>60</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -2191,18 +2194,18 @@
         <v>76</v>
       </c>
       <c r="D19" t="n">
-        <v>549.0826416015625</v>
+        <v>602.2460327148438</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6799999999999999</v>
+        <v>10.43</v>
       </c>
       <c r="F19" t="n">
-        <v>60</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -2213,18 +2216,18 @@
         <v>101</v>
       </c>
       <c r="D20" t="n">
-        <v>671.1787719726562</v>
+        <v>765.7063598632812</v>
       </c>
       <c r="E20" t="n">
-        <v>4.49</v>
+        <v>19.21</v>
       </c>
       <c r="F20" t="n">
-        <v>60</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2235,18 +2238,18 @@
         <v>225</v>
       </c>
       <c r="D21" t="n">
-        <v>4092.51123046875</v>
+        <v>9699.3623046875</v>
       </c>
       <c r="E21" t="n">
-        <v>6.05</v>
+        <v>151.34</v>
       </c>
       <c r="F21" t="n">
-        <v>60</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2257,18 +2260,18 @@
         <v>442</v>
       </c>
       <c r="D22" t="n">
-        <v>57587.23046875</v>
+        <v>221479.34375</v>
       </c>
       <c r="E22" t="n">
-        <v>13.4</v>
+        <v>336.12</v>
       </c>
       <c r="F22" t="n">
-        <v>60.03</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2279,18 +2282,18 @@
         <v>29</v>
       </c>
       <c r="D23" t="n">
-        <v>2020</v>
+        <v>2080</v>
       </c>
       <c r="E23" t="n">
-        <v>-0</v>
+        <v>2.97</v>
       </c>
       <c r="F23" t="n">
-        <v>60</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2301,18 +2304,18 @@
         <v>51</v>
       </c>
       <c r="D24" t="n">
-        <v>435.1170043945313</v>
+        <v>462.7006530761719</v>
       </c>
       <c r="E24" t="n">
-        <v>1.19</v>
+        <v>7.61</v>
       </c>
       <c r="F24" t="n">
-        <v>60</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2323,18 +2326,18 @@
         <v>52</v>
       </c>
       <c r="D25" t="n">
-        <v>7544.6630859375</v>
+        <v>8223.33203125</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
-        <v>60</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2345,18 +2348,18 @@
         <v>76</v>
       </c>
       <c r="D26" t="n">
-        <v>549.0826416015625</v>
+        <v>602.2460327148438</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6799999999999999</v>
+        <v>10.43</v>
       </c>
       <c r="F26" t="n">
-        <v>60</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2367,18 +2370,18 @@
         <v>101</v>
       </c>
       <c r="D27" t="n">
-        <v>671.1787719726562</v>
+        <v>765.7063598632812</v>
       </c>
       <c r="E27" t="n">
-        <v>4.49</v>
+        <v>19.21</v>
       </c>
       <c r="F27" t="n">
-        <v>60</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2389,18 +2392,18 @@
         <v>225</v>
       </c>
       <c r="D28" t="n">
-        <v>4099.41259765625</v>
+        <v>9699.3623046875</v>
       </c>
       <c r="E28" t="n">
-        <v>6.23</v>
+        <v>151.34</v>
       </c>
       <c r="F28" t="n">
-        <v>60</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2411,13 +2414,13 @@
         <v>442</v>
       </c>
       <c r="D29" t="n">
-        <v>58189.92578125</v>
+        <v>221479.34375</v>
       </c>
       <c r="E29" t="n">
-        <v>14.58</v>
+        <v>336.12</v>
       </c>
       <c r="F29" t="n">
-        <v>60</v>
+        <v>2.02</v>
       </c>
     </row>
   </sheetData>
@@ -2442,7 +2445,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Iterations</t>
+          <t>Timelimit</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2473,7 +2476,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2484,18 +2487,18 @@
         <v>29</v>
       </c>
       <c r="D2" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1</v>
+        <v>-0</v>
       </c>
       <c r="F2" t="n">
-        <v>20.48</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -2512,12 +2515,12 @@
         <v>2.04</v>
       </c>
       <c r="F3" t="n">
-        <v>50.49</v>
+        <v>60.06</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -2534,12 +2537,12 @@
         <v>0.06</v>
       </c>
       <c r="F4" t="n">
-        <v>50.2</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -2556,12 +2559,12 @@
         <v>1.78</v>
       </c>
       <c r="F5" t="n">
-        <v>100.73</v>
+        <v>60.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -2572,18 +2575,18 @@
         <v>101</v>
       </c>
       <c r="D6" t="n">
-        <v>677.70947265625</v>
+        <v>679.5157470703125</v>
       </c>
       <c r="E6" t="n">
-        <v>5.510000000000001</v>
+        <v>5.79</v>
       </c>
       <c r="F6" t="n">
-        <v>172.39</v>
+        <v>60.16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -2594,18 +2597,18 @@
         <v>225</v>
       </c>
       <c r="D7" t="n">
-        <v>4142.7646484375</v>
+        <v>4190.5361328125</v>
       </c>
       <c r="E7" t="n">
-        <v>7.35</v>
+        <v>8.59</v>
       </c>
       <c r="F7" t="n">
-        <v>743.63</v>
+        <v>60.49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -2616,18 +2619,18 @@
         <v>442</v>
       </c>
       <c r="D8" t="n">
-        <v>57966.69140625</v>
+        <v>62575.59375</v>
       </c>
       <c r="E8" t="n">
-        <v>14.14</v>
+        <v>23.22</v>
       </c>
       <c r="F8" t="n">
-        <v>2971.26</v>
+        <v>62.53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2638,18 +2641,18 @@
         <v>29</v>
       </c>
       <c r="D9" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1</v>
+        <v>-0</v>
       </c>
       <c r="F9" t="n">
-        <v>2.86</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -2660,18 +2663,18 @@
         <v>51</v>
       </c>
       <c r="D10" t="n">
-        <v>438.7414245605469</v>
+        <v>432.6891784667969</v>
       </c>
       <c r="E10" t="n">
-        <v>2.04</v>
+        <v>0.63</v>
       </c>
       <c r="F10" t="n">
-        <v>4.93</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -2682,18 +2685,18 @@
         <v>52</v>
       </c>
       <c r="D11" t="n">
-        <v>7548.9931640625</v>
+        <v>7544.36572265625</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06</v>
+        <v>-0</v>
       </c>
       <c r="F11" t="n">
-        <v>5.22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -2704,18 +2707,18 @@
         <v>76</v>
       </c>
       <c r="D12" t="n">
-        <v>555.097900390625</v>
+        <v>553.6527099609375</v>
       </c>
       <c r="E12" t="n">
-        <v>1.78</v>
+        <v>1.52</v>
       </c>
       <c r="F12" t="n">
-        <v>8.6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -2726,18 +2729,18 @@
         <v>101</v>
       </c>
       <c r="D13" t="n">
-        <v>677.70947265625</v>
+        <v>672.9217529296875</v>
       </c>
       <c r="E13" t="n">
-        <v>5.510000000000001</v>
+        <v>4.77</v>
       </c>
       <c r="F13" t="n">
-        <v>14.01</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -2754,12 +2757,12 @@
         <v>7.35</v>
       </c>
       <c r="F14" t="n">
-        <v>53.6</v>
+        <v>60.04</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -2770,18 +2773,18 @@
         <v>442</v>
       </c>
       <c r="D15" t="n">
-        <v>57966.69140625</v>
+        <v>58054.23046875</v>
       </c>
       <c r="E15" t="n">
-        <v>14.14</v>
+        <v>14.32</v>
       </c>
       <c r="F15" t="n">
-        <v>200.59</v>
+        <v>60.19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -2798,12 +2801,12 @@
         <v>-0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.98</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -2814,18 +2817,18 @@
         <v>51</v>
       </c>
       <c r="D17" t="n">
-        <v>442.6688537597656</v>
+        <v>433.9072570800781</v>
       </c>
       <c r="E17" t="n">
-        <v>2.95</v>
+        <v>0.91</v>
       </c>
       <c r="F17" t="n">
-        <v>1.19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -2836,18 +2839,18 @@
         <v>52</v>
       </c>
       <c r="D18" t="n">
-        <v>7681.4541015625</v>
+        <v>7544.6630859375</v>
       </c>
       <c r="E18" t="n">
-        <v>1.82</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1.28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -2858,18 +2861,18 @@
         <v>76</v>
       </c>
       <c r="D19" t="n">
-        <v>554.7601928710938</v>
+        <v>549.0826416015625</v>
       </c>
       <c r="E19" t="n">
-        <v>1.72</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>1.52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -2880,18 +2883,18 @@
         <v>101</v>
       </c>
       <c r="D20" t="n">
-        <v>680.8486328125</v>
+        <v>671.1787719726562</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>4.49</v>
       </c>
       <c r="F20" t="n">
-        <v>1.98</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2908,12 +2911,12 @@
         <v>6.05</v>
       </c>
       <c r="F21" t="n">
-        <v>6.72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2924,18 +2927,18 @@
         <v>442</v>
       </c>
       <c r="D22" t="n">
-        <v>58339.75</v>
+        <v>57587.23046875</v>
       </c>
       <c r="E22" t="n">
-        <v>14.88</v>
+        <v>13.4</v>
       </c>
       <c r="F22" t="n">
-        <v>33.44</v>
+        <v>60.03</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2952,12 +2955,12 @@
         <v>-0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2968,18 +2971,18 @@
         <v>51</v>
       </c>
       <c r="D24" t="n">
-        <v>442.6688537597656</v>
+        <v>435.1170043945313</v>
       </c>
       <c r="E24" t="n">
-        <v>2.95</v>
+        <v>1.19</v>
       </c>
       <c r="F24" t="n">
-        <v>1.63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2990,18 +2993,18 @@
         <v>52</v>
       </c>
       <c r="D25" t="n">
-        <v>7681.4541015625</v>
+        <v>7544.6630859375</v>
       </c>
       <c r="E25" t="n">
-        <v>1.82</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>1.62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -3012,18 +3015,18 @@
         <v>76</v>
       </c>
       <c r="D26" t="n">
-        <v>554.7601928710938</v>
+        <v>549.0826416015625</v>
       </c>
       <c r="E26" t="n">
-        <v>1.72</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="F26" t="n">
-        <v>2.23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -3034,18 +3037,18 @@
         <v>101</v>
       </c>
       <c r="D27" t="n">
-        <v>680.8486328125</v>
+        <v>671.1787719726562</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>4.49</v>
       </c>
       <c r="F27" t="n">
-        <v>2.37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -3056,18 +3059,18 @@
         <v>225</v>
       </c>
       <c r="D28" t="n">
-        <v>4092.51123046875</v>
+        <v>4099.41259765625</v>
       </c>
       <c r="E28" t="n">
-        <v>6.05</v>
+        <v>6.23</v>
       </c>
       <c r="F28" t="n">
-        <v>7.45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -3078,13 +3081,13 @@
         <v>442</v>
       </c>
       <c r="D29" t="n">
-        <v>57718.7734375</v>
+        <v>58189.92578125</v>
       </c>
       <c r="E29" t="n">
-        <v>13.66</v>
+        <v>14.58</v>
       </c>
       <c r="F29" t="n">
-        <v>34.87</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3109,7 +3112,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Timelimit</t>
+          <t>Iterations</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -3140,7 +3143,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3151,18 +3154,18 @@
         <v>29</v>
       </c>
       <c r="D2" t="n">
-        <v>2053</v>
+        <v>2022</v>
       </c>
       <c r="E2" t="n">
-        <v>1.63</v>
+        <v>0.1</v>
       </c>
       <c r="F2" t="n">
-        <v>60.02</v>
+        <v>10.44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -3173,18 +3176,18 @@
         <v>51</v>
       </c>
       <c r="D3" t="n">
-        <v>450.1444702148438</v>
+        <v>441.15625</v>
       </c>
       <c r="E3" t="n">
-        <v>4.69</v>
+        <v>2.6</v>
       </c>
       <c r="F3" t="n">
-        <v>60.02</v>
+        <v>25.52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -3195,18 +3198,18 @@
         <v>52</v>
       </c>
       <c r="D4" t="n">
-        <v>7809.74462890625</v>
+        <v>7548.9931640625</v>
       </c>
       <c r="E4" t="n">
-        <v>3.52</v>
+        <v>0.06</v>
       </c>
       <c r="F4" t="n">
-        <v>60.01</v>
+        <v>24.84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -3217,18 +3220,18 @@
         <v>76</v>
       </c>
       <c r="D5" t="n">
-        <v>584.7515258789062</v>
+        <v>556.9925537109375</v>
       </c>
       <c r="E5" t="n">
-        <v>7.22</v>
+        <v>2.13</v>
       </c>
       <c r="F5" t="n">
-        <v>60.03</v>
+        <v>50.53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -3239,18 +3242,18 @@
         <v>101</v>
       </c>
       <c r="D6" t="n">
-        <v>705.5875854492188</v>
+        <v>679.5157470703125</v>
       </c>
       <c r="E6" t="n">
-        <v>9.85</v>
+        <v>5.79</v>
       </c>
       <c r="F6" t="n">
-        <v>60.02</v>
+        <v>86.31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -3261,18 +3264,18 @@
         <v>225</v>
       </c>
       <c r="D7" t="n">
-        <v>15584.8916015625</v>
+        <v>4144.4560546875</v>
       </c>
       <c r="E7" t="n">
-        <v>303.86</v>
+        <v>7.399999999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>60.07</v>
+        <v>371.57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -3283,18 +3286,18 @@
         <v>442</v>
       </c>
       <c r="D8" t="n">
-        <v>630339.1875</v>
+        <v>57966.69140625</v>
       </c>
       <c r="E8" t="n">
-        <v>1141.23</v>
+        <v>14.14</v>
       </c>
       <c r="F8" t="n">
-        <v>60.13</v>
+        <v>1480.36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -3305,18 +3308,18 @@
         <v>29</v>
       </c>
       <c r="D9" t="n">
-        <v>2053</v>
+        <v>2022</v>
       </c>
       <c r="E9" t="n">
-        <v>1.63</v>
+        <v>0.1</v>
       </c>
       <c r="F9" t="n">
-        <v>60.01</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -3327,18 +3330,18 @@
         <v>51</v>
       </c>
       <c r="D10" t="n">
-        <v>450.1444702148438</v>
+        <v>441.15625</v>
       </c>
       <c r="E10" t="n">
-        <v>4.69</v>
+        <v>2.6</v>
       </c>
       <c r="F10" t="n">
-        <v>60.01</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -3349,18 +3352,18 @@
         <v>52</v>
       </c>
       <c r="D11" t="n">
-        <v>7809.74462890625</v>
+        <v>7548.9931640625</v>
       </c>
       <c r="E11" t="n">
-        <v>3.52</v>
+        <v>0.06</v>
       </c>
       <c r="F11" t="n">
-        <v>60</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -3371,18 +3374,18 @@
         <v>76</v>
       </c>
       <c r="D12" t="n">
-        <v>584.7515258789062</v>
+        <v>556.9925537109375</v>
       </c>
       <c r="E12" t="n">
-        <v>7.22</v>
+        <v>2.13</v>
       </c>
       <c r="F12" t="n">
-        <v>60.01</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -3393,18 +3396,18 @@
         <v>101</v>
       </c>
       <c r="D13" t="n">
-        <v>705.5875854492188</v>
+        <v>679.5157470703125</v>
       </c>
       <c r="E13" t="n">
-        <v>9.85</v>
+        <v>5.79</v>
       </c>
       <c r="F13" t="n">
-        <v>60.01</v>
+        <v>7.01</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -3415,18 +3418,18 @@
         <v>225</v>
       </c>
       <c r="D14" t="n">
-        <v>8063.6953125</v>
+        <v>4144.4560546875</v>
       </c>
       <c r="E14" t="n">
-        <v>108.96</v>
+        <v>7.399999999999999</v>
       </c>
       <c r="F14" t="n">
-        <v>60.06</v>
+        <v>26.83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -3437,18 +3440,18 @@
         <v>442</v>
       </c>
       <c r="D15" t="n">
-        <v>623649.25</v>
+        <v>57966.69140625</v>
       </c>
       <c r="E15" t="n">
-        <v>1128.05</v>
+        <v>14.14</v>
       </c>
       <c r="F15" t="n">
-        <v>60.04</v>
+        <v>100.76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -3459,18 +3462,18 @@
         <v>29</v>
       </c>
       <c r="D16" t="n">
-        <v>2053</v>
+        <v>2022</v>
       </c>
       <c r="E16" t="n">
-        <v>1.63</v>
+        <v>0.1</v>
       </c>
       <c r="F16" t="n">
-        <v>60.01</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -3481,18 +3484,18 @@
         <v>51</v>
       </c>
       <c r="D17" t="n">
-        <v>450.1444702148438</v>
+        <v>442.9311828613281</v>
       </c>
       <c r="E17" t="n">
-        <v>4.69</v>
+        <v>3.01</v>
       </c>
       <c r="F17" t="n">
-        <v>60.01</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -3503,18 +3506,18 @@
         <v>52</v>
       </c>
       <c r="D18" t="n">
-        <v>7809.74462890625</v>
+        <v>7731.24658203125</v>
       </c>
       <c r="E18" t="n">
-        <v>3.52</v>
+        <v>2.48</v>
       </c>
       <c r="F18" t="n">
-        <v>60.01</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -3525,18 +3528,18 @@
         <v>76</v>
       </c>
       <c r="D19" t="n">
-        <v>584.7515258789062</v>
+        <v>558.17236328125</v>
       </c>
       <c r="E19" t="n">
-        <v>7.22</v>
+        <v>2.34</v>
       </c>
       <c r="F19" t="n">
-        <v>60.01</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -3547,18 +3550,18 @@
         <v>101</v>
       </c>
       <c r="D20" t="n">
-        <v>705.5875854492188</v>
+        <v>680.8486328125</v>
       </c>
       <c r="E20" t="n">
-        <v>9.85</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
-        <v>60.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -3569,18 +3572,18 @@
         <v>225</v>
       </c>
       <c r="D21" t="n">
-        <v>6818.89697265625</v>
+        <v>4149.01708984375</v>
       </c>
       <c r="E21" t="n">
-        <v>76.7</v>
+        <v>7.52</v>
       </c>
       <c r="F21" t="n">
-        <v>60.01</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -3591,18 +3594,18 @@
         <v>442</v>
       </c>
       <c r="D22" t="n">
-        <v>623649.25</v>
+        <v>57573.203125</v>
       </c>
       <c r="E22" t="n">
-        <v>1128.05</v>
+        <v>13.37</v>
       </c>
       <c r="F22" t="n">
-        <v>60.03</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -3613,18 +3616,18 @@
         <v>29</v>
       </c>
       <c r="D23" t="n">
-        <v>2053</v>
+        <v>2022</v>
       </c>
       <c r="E23" t="n">
-        <v>1.63</v>
+        <v>0.1</v>
       </c>
       <c r="F23" t="n">
-        <v>60.02</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -3635,18 +3638,18 @@
         <v>51</v>
       </c>
       <c r="D24" t="n">
-        <v>450.1444702148438</v>
+        <v>442.9311828613281</v>
       </c>
       <c r="E24" t="n">
-        <v>4.69</v>
+        <v>3.01</v>
       </c>
       <c r="F24" t="n">
-        <v>60.02</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -3657,18 +3660,18 @@
         <v>52</v>
       </c>
       <c r="D25" t="n">
-        <v>7809.74462890625</v>
+        <v>7731.24658203125</v>
       </c>
       <c r="E25" t="n">
-        <v>3.52</v>
+        <v>2.48</v>
       </c>
       <c r="F25" t="n">
-        <v>60.01</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -3679,18 +3682,18 @@
         <v>76</v>
       </c>
       <c r="D26" t="n">
-        <v>584.7515258789062</v>
+        <v>558.17236328125</v>
       </c>
       <c r="E26" t="n">
-        <v>7.22</v>
+        <v>2.34</v>
       </c>
       <c r="F26" t="n">
-        <v>60.01</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -3701,18 +3704,18 @@
         <v>101</v>
       </c>
       <c r="D27" t="n">
-        <v>705.5875854492188</v>
+        <v>680.8486328125</v>
       </c>
       <c r="E27" t="n">
-        <v>9.85</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
-        <v>60.01</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -3723,18 +3726,18 @@
         <v>225</v>
       </c>
       <c r="D28" t="n">
-        <v>8572.080078125</v>
+        <v>4149.01708984375</v>
       </c>
       <c r="E28" t="n">
-        <v>122.13</v>
+        <v>7.52</v>
       </c>
       <c r="F28" t="n">
-        <v>60.06</v>
+        <v>3.84</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -3745,13 +3748,13 @@
         <v>442</v>
       </c>
       <c r="D29" t="n">
-        <v>623649.25</v>
+        <v>57835.9921875</v>
       </c>
       <c r="E29" t="n">
-        <v>1128.05</v>
+        <v>13.89</v>
       </c>
       <c r="F29" t="n">
-        <v>60.11</v>
+        <v>17.35</v>
       </c>
     </row>
   </sheetData>
@@ -3818,6 +3821,2007 @@
         <v>29</v>
       </c>
       <c r="D2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20.48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" t="n">
+        <v>438.7414245605469</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="F3" t="n">
+        <v>50.49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>52</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7548.9931640625</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F4" t="n">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>76</v>
+      </c>
+      <c r="D5" t="n">
+        <v>555.097900390625</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="F5" t="n">
+        <v>100.73</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>101</v>
+      </c>
+      <c r="D6" t="n">
+        <v>677.70947265625</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5.510000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>172.39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>225</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4142.7646484375</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="F7" t="n">
+        <v>743.63</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>442</v>
+      </c>
+      <c r="D8" t="n">
+        <v>57966.69140625</v>
+      </c>
+      <c r="E8" t="n">
+        <v>14.14</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2971.26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>29</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>51</v>
+      </c>
+      <c r="D10" t="n">
+        <v>438.7414245605469</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>52</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7548.9931640625</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>76</v>
+      </c>
+      <c r="D12" t="n">
+        <v>555.097900390625</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>101</v>
+      </c>
+      <c r="D13" t="n">
+        <v>677.70947265625</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.510000000000001</v>
+      </c>
+      <c r="F13" t="n">
+        <v>14.01</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>225</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4142.7646484375</v>
+      </c>
+      <c r="E14" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="F14" t="n">
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>442</v>
+      </c>
+      <c r="D15" t="n">
+        <v>57966.69140625</v>
+      </c>
+      <c r="E15" t="n">
+        <v>14.14</v>
+      </c>
+      <c r="F15" t="n">
+        <v>200.59</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>29</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>51</v>
+      </c>
+      <c r="D17" t="n">
+        <v>442.6688537597656</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>52</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7681.4541015625</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>76</v>
+      </c>
+      <c r="D19" t="n">
+        <v>554.7601928710938</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>101</v>
+      </c>
+      <c r="D20" t="n">
+        <v>680.8486328125</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>225</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4092.51123046875</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>442</v>
+      </c>
+      <c r="D22" t="n">
+        <v>58339.75</v>
+      </c>
+      <c r="E22" t="n">
+        <v>14.88</v>
+      </c>
+      <c r="F22" t="n">
+        <v>33.44</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>29</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>51</v>
+      </c>
+      <c r="D24" t="n">
+        <v>442.6688537597656</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>52</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7681.4541015625</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>76</v>
+      </c>
+      <c r="D26" t="n">
+        <v>554.7601928710938</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>101</v>
+      </c>
+      <c r="D27" t="n">
+        <v>680.8486328125</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>225</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4092.51123046875</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="F28" t="n">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>442</v>
+      </c>
+      <c r="D29" t="n">
+        <v>57718.7734375</v>
+      </c>
+      <c r="E29" t="n">
+        <v>13.66</v>
+      </c>
+      <c r="F29" t="n">
+        <v>34.87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Timelimit</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Executer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Cities</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fitness</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Gap</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>60</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>29</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2053</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="F2" t="n">
+        <v>60.02</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>60</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" t="n">
+        <v>450.1444702148438</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="F3" t="n">
+        <v>60.02</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>60</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>52</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7809.74462890625</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="F4" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>60</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>76</v>
+      </c>
+      <c r="D5" t="n">
+        <v>584.7515258789062</v>
+      </c>
+      <c r="E5" t="n">
+        <v>7.22</v>
+      </c>
+      <c r="F5" t="n">
+        <v>60.03</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>60</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>101</v>
+      </c>
+      <c r="D6" t="n">
+        <v>705.5875854492188</v>
+      </c>
+      <c r="E6" t="n">
+        <v>9.85</v>
+      </c>
+      <c r="F6" t="n">
+        <v>60.02</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>60</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>225</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15584.8916015625</v>
+      </c>
+      <c r="E7" t="n">
+        <v>303.86</v>
+      </c>
+      <c r="F7" t="n">
+        <v>60.07</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>60</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>442</v>
+      </c>
+      <c r="D8" t="n">
+        <v>630339.1875</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1141.23</v>
+      </c>
+      <c r="F8" t="n">
+        <v>60.13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>60</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>29</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2053</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="F9" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>60</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>51</v>
+      </c>
+      <c r="D10" t="n">
+        <v>450.1444702148438</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="F10" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>60</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>52</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7809.74462890625</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="F11" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>60</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>76</v>
+      </c>
+      <c r="D12" t="n">
+        <v>584.7515258789062</v>
+      </c>
+      <c r="E12" t="n">
+        <v>7.22</v>
+      </c>
+      <c r="F12" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>101</v>
+      </c>
+      <c r="D13" t="n">
+        <v>705.5875854492188</v>
+      </c>
+      <c r="E13" t="n">
+        <v>9.85</v>
+      </c>
+      <c r="F13" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>225</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8063.6953125</v>
+      </c>
+      <c r="E14" t="n">
+        <v>108.96</v>
+      </c>
+      <c r="F14" t="n">
+        <v>60.06</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>60</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>442</v>
+      </c>
+      <c r="D15" t="n">
+        <v>623649.25</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1128.05</v>
+      </c>
+      <c r="F15" t="n">
+        <v>60.04</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>60</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>29</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2053</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="F16" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>51</v>
+      </c>
+      <c r="D17" t="n">
+        <v>450.1444702148438</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="F17" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>60</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>52</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7809.74462890625</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="F18" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>60</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>76</v>
+      </c>
+      <c r="D19" t="n">
+        <v>584.7515258789062</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7.22</v>
+      </c>
+      <c r="F19" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>60</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>101</v>
+      </c>
+      <c r="D20" t="n">
+        <v>705.5875854492188</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9.85</v>
+      </c>
+      <c r="F20" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>60</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>225</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6818.89697265625</v>
+      </c>
+      <c r="E21" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="F21" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>60</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>442</v>
+      </c>
+      <c r="D22" t="n">
+        <v>623649.25</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1128.05</v>
+      </c>
+      <c r="F22" t="n">
+        <v>60.03</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>60</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>29</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2053</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="F23" t="n">
+        <v>60.02</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>60</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>51</v>
+      </c>
+      <c r="D24" t="n">
+        <v>450.1444702148438</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="F24" t="n">
+        <v>60.02</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>60</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>52</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7809.74462890625</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="F25" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>60</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>76</v>
+      </c>
+      <c r="D26" t="n">
+        <v>584.7515258789062</v>
+      </c>
+      <c r="E26" t="n">
+        <v>7.22</v>
+      </c>
+      <c r="F26" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>60</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>101</v>
+      </c>
+      <c r="D27" t="n">
+        <v>705.5875854492188</v>
+      </c>
+      <c r="E27" t="n">
+        <v>9.85</v>
+      </c>
+      <c r="F27" t="n">
+        <v>60.01</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>60</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>225</v>
+      </c>
+      <c r="D28" t="n">
+        <v>8572.080078125</v>
+      </c>
+      <c r="E28" t="n">
+        <v>122.13</v>
+      </c>
+      <c r="F28" t="n">
+        <v>60.06</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>60</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>442</v>
+      </c>
+      <c r="D29" t="n">
+        <v>623649.25</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1128.05</v>
+      </c>
+      <c r="F29" t="n">
+        <v>60.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Iterations</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Executer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Cities</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fitness</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Gap</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>500</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>29</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2101</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10.38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>500</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" t="n">
+        <v>465.7870178222656</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="F3" t="n">
+        <v>12.88</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>500</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>52</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7737.705078125</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="F4" t="n">
+        <v>14.84</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>500</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>76</v>
+      </c>
+      <c r="D5" t="n">
+        <v>597.7548217773438</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>18.42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>500</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>101</v>
+      </c>
+      <c r="D6" t="n">
+        <v>687.9953002929688</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7.109999999999999</v>
+      </c>
+      <c r="F6" t="n">
+        <v>25.28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>500</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>225</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15489.15234375</v>
+      </c>
+      <c r="E7" t="n">
+        <v>301.38</v>
+      </c>
+      <c r="F7" t="n">
+        <v>54.8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>500</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>442</v>
+      </c>
+      <c r="D8" t="n">
+        <v>435430.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>757.4200000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>106.7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>500</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>29</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2101</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="F9" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>500</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>51</v>
+      </c>
+      <c r="D10" t="n">
+        <v>465.7870178222656</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10.03</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>500</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>52</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7737.705078125</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>500</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>76</v>
+      </c>
+      <c r="D12" t="n">
+        <v>597.7548217773438</v>
+      </c>
+      <c r="E12" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>500</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>101</v>
+      </c>
+      <c r="D13" t="n">
+        <v>687.9953002929688</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7.109999999999999</v>
+      </c>
+      <c r="F13" t="n">
+        <v>15.42</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>500</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>225</v>
+      </c>
+      <c r="D14" t="n">
+        <v>15489.15234375</v>
+      </c>
+      <c r="E14" t="n">
+        <v>301.38</v>
+      </c>
+      <c r="F14" t="n">
+        <v>31.35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>500</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>multi</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>442</v>
+      </c>
+      <c r="D15" t="n">
+        <v>435430.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>757.4200000000001</v>
+      </c>
+      <c r="F15" t="n">
+        <v>61.78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>500</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>29</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2101</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>500</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>51</v>
+      </c>
+      <c r="D17" t="n">
+        <v>465.7870178222656</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="F17" t="n">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>500</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>52</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7737.705078125</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10.02</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>500</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>76</v>
+      </c>
+      <c r="D19" t="n">
+        <v>597.7548217773438</v>
+      </c>
+      <c r="E19" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="F19" t="n">
+        <v>10.69</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>500</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>101</v>
+      </c>
+      <c r="D20" t="n">
+        <v>687.9953002929688</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7.109999999999999</v>
+      </c>
+      <c r="F20" t="n">
+        <v>14.62</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>500</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>225</v>
+      </c>
+      <c r="D21" t="n">
+        <v>15489.15234375</v>
+      </c>
+      <c r="E21" t="n">
+        <v>301.38</v>
+      </c>
+      <c r="F21" t="n">
+        <v>29.61</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>500</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>gpu</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>442</v>
+      </c>
+      <c r="D22" t="n">
+        <v>435430.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>757.4200000000001</v>
+      </c>
+      <c r="F22" t="n">
+        <v>60.99</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>500</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>29</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2101</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10.13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>500</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>51</v>
+      </c>
+      <c r="D24" t="n">
+        <v>465.7870178222656</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="F24" t="n">
+        <v>10.38</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>500</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>52</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7737.705078125</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="F25" t="n">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>500</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>76</v>
+      </c>
+      <c r="D26" t="n">
+        <v>597.7548217773438</v>
+      </c>
+      <c r="E26" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="F26" t="n">
+        <v>11.67</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>500</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>101</v>
+      </c>
+      <c r="D27" t="n">
+        <v>687.9953002929688</v>
+      </c>
+      <c r="E27" t="n">
+        <v>7.109999999999999</v>
+      </c>
+      <c r="F27" t="n">
+        <v>15.71</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>500</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>225</v>
+      </c>
+      <c r="D28" t="n">
+        <v>15489.15234375</v>
+      </c>
+      <c r="E28" t="n">
+        <v>301.38</v>
+      </c>
+      <c r="F28" t="n">
+        <v>31.22</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>500</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>442</v>
+      </c>
+      <c r="D29" t="n">
+        <v>435430.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>757.4200000000001</v>
+      </c>
+      <c r="F29" t="n">
+        <v>70.39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Iterations</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Executer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Cities</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fitness</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Gap</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>29</v>
+      </c>
+      <c r="D2" t="n">
         <v>2097</v>
       </c>
       <c r="E2" t="n">

</xml_diff>